<commit_message>
adding filter, update search, update relasi kat_soal, sorting asc desc
</commit_message>
<xml_diff>
--- a/public/sample/import-peserta.xlsx
+++ b/public/sample/import-peserta.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24334"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project-Coding\aplikasi-ujian-online\public\sample\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14E7336D-6E1C-4C6F-A24A-C6647836BEA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{958FD5D8-3243-4DCA-AC98-445091CFA6C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1116" yWindow="1116" windowWidth="17280" windowHeight="8880" xr2:uid="{A42551A4-E829-4EFF-ABAD-9AFD4A94D21A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A42551A4-E829-4EFF-ABAD-9AFD4A94D21A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="13">
   <si>
     <t>nis</t>
   </si>
@@ -57,20 +57,38 @@
     <t>status</t>
   </si>
   <si>
-    <t>cekfix-1</t>
-  </si>
-  <si>
-    <t>cekfix-2</t>
+    <t>peserta-1</t>
+  </si>
+  <si>
+    <t>peserta-2</t>
+  </si>
+  <si>
+    <t>filter</t>
+  </si>
+  <si>
+    <t>peserta-3</t>
+  </si>
+  <si>
+    <t>peserta-4</t>
+  </si>
+  <si>
+    <t>peserta-5</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -412,22 +430,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12F15DB0-C0ED-4325-90CA-29475FBAD9B5}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.33203125" customWidth="1"/>
-    <col min="3" max="3" width="16.44140625" customWidth="1"/>
-    <col min="5" max="5" width="18.5546875" customWidth="1"/>
+    <col min="3" max="3" width="9.44140625" customWidth="1"/>
+    <col min="5" max="5" width="12.44140625" customWidth="1"/>
     <col min="6" max="6" width="11.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -446,8 +464,11 @@
       <c r="F1" t="s">
         <v>4</v>
       </c>
+      <c r="G1" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -461,13 +482,16 @@
         <v>1</v>
       </c>
       <c r="E2">
-        <v>99999999</v>
+        <v>11111111</v>
       </c>
       <c r="F2" t="s">
         <v>7</v>
       </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -478,16 +502,89 @@
         <v>0</v>
       </c>
       <c r="D3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E3">
-        <v>91919191</v>
+        <v>22222222</v>
       </c>
       <c r="F3" t="s">
         <v>8</v>
       </c>
+      <c r="G3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>33333333</v>
+      </c>
+      <c r="F4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="E5">
+        <v>44444444</v>
+      </c>
+      <c r="F5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>55555555</v>
+      </c>
+      <c r="F6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>